<commit_message>
añadida mecanica y animaciones de disparo para el enemigo DroidArmed pero por algun motivo solo 1 de las 3 balas que salen disparadas por 3 driodes distintos restan vidas al player, ademas no siempre una de estas balas le resta vida ademas el spawn de la bala no esta en el sitio correcto y hay que mirarlo, eso hay que solucionarlo. Pero al menos los robots ya tienen animacion de disparo que se activa solo si ven al player y sale un proyectil del robot que quita vida al player
</commit_message>
<xml_diff>
--- a/Listado_De_Tareas-Red_Pill.xlsx
+++ b/Listado_De_Tareas-Red_Pill.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="183">
   <si>
     <t>ID</t>
   </si>
@@ -418,7 +418,7 @@
     <t>media</t>
   </si>
   <si>
-    <t>Animaciones Robot Desarmado</t>
+    <t>Animaciones Cyborg</t>
   </si>
   <si>
     <t>Animaciones para El obstaculo dinamico cyborg</t>
@@ -442,40 +442,46 @@
     <t xml:space="preserve"> Crear o buscar las texturas del obstaculo dinamico Robot desarmado </t>
   </si>
   <si>
-    <t>Comportamiento Robot desarmado</t>
+    <t>Comportamiento Robot Armado</t>
   </si>
   <si>
     <t>Programar el comportamiento de este obstaculo dinamico Robot desarmado</t>
   </si>
   <si>
+    <t>Animaciones robot desarmado</t>
+  </si>
+  <si>
+    <t>Animaciones para El obstaculo dinamico robot desarmado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En curso </t>
+  </si>
+  <si>
+    <t>Robots Armados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crear o buscar un modelo para el obstaculo dinamico Robot armado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No creo que sea complicado encontrar un buen modelo de un robot armado. </t>
+  </si>
+  <si>
+    <t>Robot armado Texturas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crear o buscar las texturas del obstaculo dinamico Robot armado </t>
+  </si>
+  <si>
+    <t>Comportamiento Robot armado</t>
+  </si>
+  <si>
+    <t>Programar el comportamiento de este obstaculo dinamico Robot armado</t>
+  </si>
+  <si>
+    <t>E de hacer que si ve al jugador incie la animacion de disparo y salga un disparo…</t>
+  </si>
+  <si>
     <t>Animaciones robot armado</t>
-  </si>
-  <si>
-    <t>Animaciones para El obstaculo dinamico robot desarmado</t>
-  </si>
-  <si>
-    <t>Robots Armados</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Crear o buscar un modelo para el obstaculo dinamico Robot armado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No creo que sea complicado encontrar un buen modelo de un robot armado. </t>
-  </si>
-  <si>
-    <t>Robot armado Texturas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Crear o buscar las texturas del obstaculo dinamico Robot armado </t>
-  </si>
-  <si>
-    <t>Comportamiento Robot armado</t>
-  </si>
-  <si>
-    <t>Programar el comportamiento de este obstaculo dinamico Robot armado</t>
-  </si>
-  <si>
-    <t>E de hacer que si ve al jugador incie la animacion de disparo y salga un disparo…</t>
   </si>
   <si>
     <t>Animaciones para El obstaculo dinamico robot armado</t>
@@ -580,7 +586,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -771,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -797,9 +802,6 @@
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -814,17 +816,17 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="5" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="5" fillId="7" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="5" fillId="8" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1116,7 +1118,6 @@
     <col customWidth="1" min="7" max="7" width="15.38"/>
     <col customWidth="1" min="8" max="8" width="15.13"/>
     <col customWidth="1" min="9" max="9" width="255.75"/>
-    <col customWidth="1" min="10" max="26" width="12.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1199,10 +1200,10 @@
       <c r="G3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1210,28 +1211,28 @@
       <c r="A4" s="4">
         <v>3.0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1257,10 +1258,10 @@
       <c r="G5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1268,28 +1269,28 @@
       <c r="A6" s="4">
         <v>5.0</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1318,12 +1319,12 @@
       <c r="H7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1350,51 +1351,51 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1420,10 +1421,10 @@
       <c r="G12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1449,10 +1450,10 @@
       <c r="G13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1478,10 +1479,10 @@
       <c r="G14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1489,117 +1490,117 @@
       <c r="A15" s="6">
         <v>10.0</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="10"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1610,25 +1611,25 @@
       <c r="B21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1636,28 +1637,28 @@
       <c r="A22" s="6">
         <v>12.0</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1665,28 +1666,28 @@
       <c r="A23" s="4">
         <v>13.0</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1694,28 +1695,28 @@
       <c r="A24" s="6">
         <v>14.0</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="16" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1723,104 +1724,104 @@
       <c r="A25" s="4">
         <v>15.0</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="20" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1828,28 +1829,28 @@
       <c r="A30" s="4">
         <v>16.0</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1857,28 +1858,28 @@
       <c r="A31" s="6">
         <v>17.0</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1886,28 +1887,28 @@
       <c r="A32" s="4">
         <v>18.0</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1915,28 +1916,28 @@
       <c r="A33" s="6">
         <v>19.0</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="13" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1944,28 +1945,28 @@
       <c r="A34" s="4">
         <v>20.0</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1973,28 +1974,28 @@
       <c r="A35" s="4">
         <v>21.0</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2002,28 +2003,28 @@
       <c r="A36" s="6">
         <v>22.0</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2031,28 +2032,28 @@
       <c r="A37" s="4">
         <v>23.0</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="13" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2060,28 +2061,28 @@
       <c r="A38" s="6">
         <v>24.0</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2089,104 +2090,104 @@
       <c r="A39" s="4">
         <v>25.0</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="13" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="14"/>
-      <c r="B40" s="20" t="s">
+      <c r="A40" s="13"/>
+      <c r="B40" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="I40" s="17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="14"/>
-      <c r="B43" s="21" t="s">
+      <c r="A43" s="13"/>
+      <c r="B43" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="21" t="s">
+      <c r="I43" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2215,7 +2216,7 @@
       <c r="H44" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="10" t="s">
+      <c r="I44" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2244,7 +2245,7 @@
       <c r="H45" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I45" s="9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2270,99 +2271,99 @@
       <c r="G46" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="H46" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I46" s="10" t="s">
+      <c r="I46" s="9" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="14"/>
-      <c r="B47" s="21" t="s">
+      <c r="A47" s="13"/>
+      <c r="B47" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="I47" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="14"/>
-      <c r="B50" s="22" t="s">
+      <c r="A50" s="13"/>
+      <c r="B50" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="E50" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="22" t="s">
+      <c r="H50" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I50" s="22" t="s">
+      <c r="I50" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="6">
@@ -2386,10 +2387,10 @@
       <c r="G52" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H52" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I52" s="10" t="s">
+      <c r="I52" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2415,10 +2416,10 @@
       <c r="G53" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H53" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I53" s="10" t="s">
+      <c r="I53" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2426,55 +2427,55 @@
       <c r="A54" s="4">
         <v>31.0</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H54" s="16" t="s">
+      <c r="H54" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I54" s="14"/>
+      <c r="I54" s="13"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="6">
         <v>32.0</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H55" s="16" t="s">
+      <c r="H55" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I55" s="14" t="s">
+      <c r="I55" s="13" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2500,10 +2501,10 @@
       <c r="G56" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="I56" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2529,10 +2530,10 @@
       <c r="G57" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H57" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="I57" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2540,55 +2541,55 @@
       <c r="A58" s="4">
         <v>35.0</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H58" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I58" s="14"/>
+      <c r="H58" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="13"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="4">
         <v>36.0</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F59" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H59" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I59" s="14" t="s">
+      <c r="H59" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I59" s="13" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2597,10 +2598,10 @@
         <v>37.0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>32</v>
@@ -2614,11 +2615,11 @@
       <c r="G60" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H60" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>149</v>
+      <c r="H60" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -2626,10 +2627,10 @@
         <v>38.0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>32</v>
@@ -2643,10 +2644,10 @@
       <c r="G61" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H61" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I61" s="10" t="s">
+      <c r="H61" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2654,58 +2655,58 @@
       <c r="A62" s="6">
         <v>39.0</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="C62" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D62" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F62" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G62" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H62" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I62" s="14" t="s">
-        <v>154</v>
+      <c r="H62" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="4">
         <v>40.0</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="14" t="s">
+      <c r="B63" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F63" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H63" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>156</v>
+      <c r="H63" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -2713,10 +2714,10 @@
         <v>41.0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>32</v>
@@ -2730,69 +2731,69 @@
       <c r="G64" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H64" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I64" s="10" t="s">
-        <v>160</v>
+      <c r="H64" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="6">
         <v>42.0</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H65" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>163</v>
+      <c r="I65" s="13" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="4">
         <v>43.0</v>
       </c>
-      <c r="B66" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="D66" s="14" t="s">
+      <c r="B66" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G66" s="14" t="s">
+      <c r="G66" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H66" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>166</v>
+      <c r="H66" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -2800,10 +2801,10 @@
         <v>44.0</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>32</v>
@@ -2817,11 +2818,11 @@
       <c r="G67" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H67" s="9" t="s">
+      <c r="H67" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I67" s="10" t="s">
-        <v>169</v>
+      <c r="I67" s="9" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -2829,10 +2830,10 @@
         <v>45.0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>32</v>
@@ -2846,95 +2847,95 @@
       <c r="G68" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H68" s="9" t="s">
+      <c r="H68" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="10" t="s">
-        <v>172</v>
+      <c r="I68" s="9" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="4">
         <v>46.0</v>
       </c>
-      <c r="B69" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" s="14" t="s">
+      <c r="B69" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D69" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E69" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="G69" s="14" t="s">
+      <c r="E69" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G69" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H69" s="16" t="s">
+      <c r="H69" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I69" s="14" t="s">
-        <v>176</v>
+      <c r="I69" s="13" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="6">
         <v>47.0</v>
       </c>
-      <c r="B70" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D70" s="14" t="s">
+      <c r="B70" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F70" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G70" s="14" t="s">
+      <c r="G70" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H70" s="16" t="s">
+      <c r="H70" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I70" s="14" t="s">
-        <v>179</v>
+      <c r="I70" s="13" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="14"/>
-      <c r="B71" s="22" t="s">
+      <c r="A71" s="13"/>
+      <c r="B71" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D71" s="22" t="s">
+      <c r="C71" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E71" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="22" t="s">
+      <c r="F71" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G71" s="22" t="s">
+      <c r="G71" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H71" s="22" t="s">
+      <c r="H71" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I71" s="22" t="s">
+      <c r="I71" s="19" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>